<commit_message>
change commtype to intergerfield
</commit_message>
<xml_diff>
--- a/futures/management/fixtures/root_symbols.xlsx
+++ b/futures/management/fixtures/root_symbols.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="268">
   <si>
     <t>A.DCE</t>
   </si>
@@ -835,51 +835,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>commission</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1223,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K66" sqref="K66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1268,7 +1224,7 @@
         <v>69</v>
       </c>
       <c r="J1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>128</v>
@@ -1305,8 +1261,8 @@
       <c r="J2" s="2">
         <v>9.2E-5</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>267</v>
+      <c r="K2" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1340,8 +1296,8 @@
       <c r="J3" s="2">
         <v>9.2E-5</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>267</v>
+      <c r="K3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1375,8 +1331,8 @@
       <c r="J4" s="2">
         <v>9.2E-5</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>268</v>
+      <c r="K4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1410,8 +1366,8 @@
       <c r="J5" s="1">
         <v>13.3</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>273</v>
+      <c r="K5" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1445,8 +1401,8 @@
       <c r="J6" s="1">
         <v>13.3</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>273</v>
+      <c r="K6" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1480,8 +1436,8 @@
       <c r="J7" s="1">
         <v>13.3</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>274</v>
+      <c r="K7" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1515,8 +1471,8 @@
       <c r="J8" s="1">
         <v>20</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>275</v>
+      <c r="K8" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1550,8 +1506,8 @@
       <c r="J9" s="1">
         <v>17.2</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>274</v>
+      <c r="K9" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1585,8 +1541,8 @@
       <c r="J10" s="1">
         <v>12</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>276</v>
+      <c r="K10" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1620,8 +1576,8 @@
       <c r="J11" s="1">
         <v>16</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>273</v>
+      <c r="K11" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1655,8 +1611,8 @@
       <c r="J12" s="1">
         <v>12</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>277</v>
+      <c r="K12" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1690,8 +1646,8 @@
       <c r="J13" s="1">
         <v>12</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>273</v>
+      <c r="K13" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1725,8 +1681,8 @@
       <c r="J14" s="1">
         <v>12</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>273</v>
+      <c r="K14" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1760,8 +1716,8 @@
       <c r="J15" s="1">
         <v>8</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>273</v>
+      <c r="K15" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1795,8 +1751,8 @@
       <c r="J16" s="1">
         <v>8</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>273</v>
+      <c r="K16" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1830,8 +1786,8 @@
       <c r="J17" s="1">
         <v>20</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>276</v>
+      <c r="K17" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1865,8 +1821,8 @@
       <c r="J18" s="1">
         <v>10</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>277</v>
+      <c r="K18" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1900,8 +1856,8 @@
       <c r="J19" s="1">
         <v>6</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>274</v>
+      <c r="K19" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1935,8 +1891,8 @@
       <c r="J20" s="1">
         <v>8</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>275</v>
+      <c r="K20" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1970,8 +1926,8 @@
       <c r="J21" s="1">
         <v>14</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>278</v>
+      <c r="K21" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -2005,8 +1961,8 @@
       <c r="J22" s="1">
         <v>12</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>274</v>
+      <c r="K22" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -2040,8 +1996,8 @@
       <c r="J23" s="1">
         <v>12</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>273</v>
+      <c r="K23" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -2075,8 +2031,8 @@
       <c r="J24" s="1">
         <v>12</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>274</v>
+      <c r="K24" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -2110,8 +2066,8 @@
       <c r="J25" s="1">
         <v>12</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>277</v>
+      <c r="K25" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -2145,8 +2101,8 @@
       <c r="J26" s="1">
         <v>20</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>277</v>
+      <c r="K26" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -2180,8 +2136,8 @@
       <c r="J27" s="1">
         <v>20</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>273</v>
+      <c r="K27" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -2215,8 +2171,8 @@
       <c r="J28" s="1">
         <v>16</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>277</v>
+      <c r="K28" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -2250,8 +2206,8 @@
       <c r="J29" s="1">
         <v>8</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>278</v>
+      <c r="K29" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -2285,8 +2241,8 @@
       <c r="J30" s="1">
         <v>8</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>275</v>
+      <c r="K30" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2320,8 +2276,8 @@
       <c r="J31">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>268</v>
+      <c r="K31" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -2355,8 +2311,8 @@
       <c r="J32" s="1">
         <v>4.8</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>278</v>
+      <c r="K32" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2390,8 +2346,8 @@
       <c r="J33" s="1">
         <v>6</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>278</v>
+      <c r="K33" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2425,8 +2381,8 @@
       <c r="J34" s="1">
         <v>24</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>278</v>
+      <c r="K34" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2460,8 +2416,8 @@
       <c r="J35" s="1">
         <v>16</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>278</v>
+      <c r="K35" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -2495,8 +2451,8 @@
       <c r="J36">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>268</v>
+      <c r="K36" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -2530,8 +2486,8 @@
       <c r="J37">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>268</v>
+      <c r="K37" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2565,8 +2521,8 @@
       <c r="J38">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>268</v>
+      <c r="K38" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2600,8 +2556,8 @@
       <c r="J39">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>268</v>
+      <c r="K39" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2635,8 +2591,8 @@
       <c r="J40">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>268</v>
+      <c r="K40" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2670,8 +2626,8 @@
       <c r="J41" s="1">
         <v>8</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>278</v>
+      <c r="K41" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2705,8 +2661,8 @@
       <c r="J42" s="1">
         <v>6</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>278</v>
+      <c r="K42" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2740,8 +2696,8 @@
       <c r="J43" s="1">
         <v>10</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>278</v>
+      <c r="K43" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2775,8 +2731,8 @@
       <c r="J44" s="1">
         <v>6</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>278</v>
+      <c r="K44" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -2810,8 +2766,8 @@
       <c r="J45">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>268</v>
+      <c r="K45" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2845,8 +2801,8 @@
       <c r="J46" s="1">
         <v>16</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>278</v>
+      <c r="K46" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2880,8 +2836,8 @@
       <c r="J47" s="1">
         <v>8</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>278</v>
+      <c r="K47" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2915,8 +2871,8 @@
       <c r="J48" s="1">
         <v>10</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>278</v>
+      <c r="K48" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2950,8 +2906,8 @@
       <c r="J49" s="1">
         <v>40</v>
       </c>
-      <c r="K49" s="3" t="s">
-        <v>278</v>
+      <c r="K49" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2985,8 +2941,8 @@
       <c r="J50" s="1">
         <v>80</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>278</v>
+      <c r="K50" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -3020,8 +2976,8 @@
       <c r="J51" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>267</v>
+      <c r="K51" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -3055,8 +3011,8 @@
       <c r="J52" s="1">
         <v>12</v>
       </c>
-      <c r="K52" s="3" t="s">
-        <v>278</v>
+      <c r="K52" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -3090,8 +3046,8 @@
       <c r="J53" s="1">
         <v>40</v>
       </c>
-      <c r="K53" s="3" t="s">
-        <v>278</v>
+      <c r="K53" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -3125,8 +3081,8 @@
       <c r="J54">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>269</v>
+      <c r="K54" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3160,8 +3116,8 @@
       <c r="J55" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="K55" s="3" t="s">
-        <v>267</v>
+      <c r="K55" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -3195,8 +3151,8 @@
       <c r="J56" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="K56" s="3" t="s">
-        <v>267</v>
+      <c r="K56" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -3230,8 +3186,8 @@
       <c r="J57" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K57" s="3" t="s">
-        <v>271</v>
+      <c r="K57" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3265,8 +3221,8 @@
       <c r="J58" s="1">
         <v>24</v>
       </c>
-      <c r="K58" s="3" t="s">
-        <v>278</v>
+      <c r="K58" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -3300,8 +3256,8 @@
       <c r="J59" s="1">
         <v>1.6000000000000001E-4</v>
       </c>
-      <c r="K59" s="3" t="s">
-        <v>270</v>
+      <c r="K59" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -3335,8 +3291,8 @@
       <c r="J60" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K60" s="3" t="s">
-        <v>270</v>
+      <c r="K60" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3370,8 +3326,8 @@
       <c r="J61" s="1">
         <v>1.8000000000000001E-4</v>
       </c>
-      <c r="K61" s="3" t="s">
-        <v>270</v>
+      <c r="K61" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3405,8 +3361,8 @@
       <c r="J62" s="1">
         <v>12</v>
       </c>
-      <c r="K62" s="3" t="s">
-        <v>278</v>
+      <c r="K62" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -3440,8 +3396,8 @@
       <c r="J63" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="K63" s="3" t="s">
-        <v>267</v>
+      <c r="K63" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -3475,8 +3431,8 @@
       <c r="J64" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="K64" s="3" t="s">
-        <v>267</v>
+      <c r="K64" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -3510,8 +3466,8 @@
       <c r="J65" s="1">
         <v>1.6000000000000001E-4</v>
       </c>
-      <c r="K65" s="3" t="s">
-        <v>267</v>
+      <c r="K65" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -3545,8 +3501,8 @@
       <c r="J66" s="1">
         <v>12</v>
       </c>
-      <c r="K66" s="3" t="s">
-        <v>278</v>
+      <c r="K66" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comminfo static file
</commit_message>
<xml_diff>
--- a/futures/management/fixtures/root_symbols.xlsx
+++ b/futures/management/fixtures/root_symbols.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$66</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1179,23 +1179,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.58203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.08203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>11</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>59</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>62</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>58</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>37</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>41</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>45</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>44</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>0.05</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J15" s="1">
         <v>8</v>
@@ -1720,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>34</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0.05</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J16" s="1">
         <v>8</v>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>31</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>35</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>0.05</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>38</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>39</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>64</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>46</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>47</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>63</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>36</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0.05</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J27" s="1">
         <v>20</v>
@@ -2140,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>50</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>0.05</v>
       </c>
       <c r="I28" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J28" s="1">
         <v>16</v>
@@ -2175,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>53</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>56</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>68</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>66</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>54</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>51</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>40</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>52</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>48</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>23</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>25</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>69</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>55</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>70</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>29</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>6</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>26</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>22</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>17</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>28</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>71</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>16</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>20</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>57</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>60</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>43</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>32</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>65</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>67</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>33</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>27</v>
       </c>

</xml_diff>